<commit_message>
Added Design for various pages
Added Design for Home , Signup and Start Page. Also iadded caption in the profile file
</commit_message>
<xml_diff>
--- a/Files/db_details.xlsx
+++ b/Files/db_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Desktop\5th Sem\WP\WP Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF07D4DA-5083-4730-ACE9-63AB468D82B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2F4336-8129-47E4-AD96-37AFAF496EF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5772" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{0DF4FBF9-D423-45E6-B3B6-6D688D385B8D}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{0DF4FBF9-D423-45E6-B3B6-6D688D385B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Images</t>
+  </si>
+  <si>
+    <t>Caption</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1BBE82-7703-4393-91A5-55700EA61214}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,14 +441,15 @@
     <col min="4" max="4" width="25.44140625" customWidth="1"/>
     <col min="5" max="5" width="20.109375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -459,12 +463,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,13 +484,16 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -494,7 +501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -502,7 +509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -510,7 +517,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>